<commit_message>
reduced params and edited batch mode to require fewer params for consistency
</commit_message>
<xml_diff>
--- a/inst/extdata/parameters.xlsx
+++ b/inst/extdata/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kluesner/Desktop/Research/For Others/James Thomas/example_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremychacon/Dropbox/RIS/projects/multieditR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649B620D-DBD5-2042-92B0-8F2AE2ACB7FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53182C2A-7722-F54A-8E87-A70EA39EB515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="2220" windowWidth="17220" windowHeight="11780" xr2:uid="{5DC8A414-0A15-2B42-9817-CC62D9680170}"/>
   </bookViews>
@@ -25,25 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
-  <si>
-    <t>Sample Name</t>
-  </si>
-  <si>
-    <t>Sample File</t>
-  </si>
-  <si>
-    <t>Control File</t>
-  </si>
-  <si>
-    <t>sgRNA</t>
-  </si>
-  <si>
-    <t>Control file is .fasta</t>
-  </si>
-  <si>
-    <t>P-value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>Test1</t>
   </si>
@@ -93,21 +75,9 @@
     <t>G</t>
   </si>
   <si>
-    <t>Edited base (e.g. "G" or "G|C")</t>
-  </si>
-  <si>
-    <t>WT base (e.g. "A")</t>
-  </si>
-  <si>
     <t>CCATCTCTAACAAAAATACG</t>
   </si>
   <si>
-    <t>sample and control file in same orientation</t>
-  </si>
-  <si>
-    <t>sgRNA in same orientation as sample file</t>
-  </si>
-  <si>
     <t>4 Round 1_B01.ab1</t>
   </si>
   <si>
@@ -127,6 +97,33 @@
   </si>
   <si>
     <t>Test10</t>
+  </si>
+  <si>
+    <t>sample_name</t>
+  </si>
+  <si>
+    <t>sample_file</t>
+  </si>
+  <si>
+    <t>ctrl_file</t>
+  </si>
+  <si>
+    <t>motif</t>
+  </si>
+  <si>
+    <t>motif_fwd</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>p_value</t>
+  </si>
+  <si>
+    <t>phred_cutoff</t>
   </si>
 </sst>
 </file>
@@ -190,9 +187,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -230,7 +227,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -336,7 +333,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -478,7 +475,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -486,11 +483,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE5656A-6A32-8B49-8F45-780B1A222171}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -501,360 +496,325 @@
     <col min="5" max="5" width="35.6640625" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
     <col min="7" max="7" width="27.5" customWidth="1"/>
-    <col min="8" max="8" width="36.83203125" customWidth="1"/>
-    <col min="9" max="9" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="b">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>0.01</v>
+      </c>
+      <c r="I2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>0.01</v>
+      </c>
+      <c r="I3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>0.01</v>
+      </c>
+      <c r="I4">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>0.01</v>
+      </c>
+      <c r="I5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>0.01</v>
+      </c>
+      <c r="I6">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>0.01</v>
+      </c>
+      <c r="I7">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>0.01</v>
+      </c>
+      <c r="I8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>0.01</v>
+      </c>
+      <c r="I9">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="H10">
+        <v>0.01</v>
+      </c>
+      <c r="I10">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>0.01</v>
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>0.01</v>
+      </c>
+      <c r="I11">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>